<commit_message>
Agrega indicadores y formato cap 5
</commit_message>
<xml_diff>
--- a/Codigo/Bases/datos_administrativos/Indicadores_de_Género/PARTICIPACIÓN_SOCIOPOLÍTICA/Consejos.xlsx
+++ b/Codigo/Bases/datos_administrativos/Indicadores_de_Género/PARTICIPACIÓN_SOCIOPOLÍTICA/Consejos.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pgalvez\OneDrive - ine.gob.gt\Documentos\GitHub\CompendioGenero2023\Codigo\Bases\datos_administrativos\Indicadores_de_Género\PARTICIPACIÓN_SOCIOPOLÍTICA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE039BA-D3D3-4923-8FEF-8467521A30E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA00B5C-82FD-42E2-AB79-890A0A704F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{5C412245-B62B-4600-B786-C7A1D1A702D5}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5C412245-B62B-4600-B786-C7A1D1A702D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Consejos" sheetId="5" r:id="rId1"/>
-    <sheet name="Consejos18-19" sheetId="7" r:id="rId2"/>
-    <sheet name="Consejos20-21" sheetId="8" r:id="rId3"/>
-    <sheet name="Consejos22" sheetId="9" r:id="rId4"/>
+    <sheet name="ConsejosSuma1" sheetId="10" r:id="rId2"/>
+    <sheet name="ConsejosSuma" sheetId="11" r:id="rId3"/>
+    <sheet name="Consejos18-19" sheetId="7" r:id="rId4"/>
+    <sheet name="Consejos20-21" sheetId="8" r:id="rId5"/>
+    <sheet name="Consejos22" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="31">
   <si>
     <t>CONADUR</t>
   </si>
@@ -167,8 +169,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,7 +494,7 @@
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:U1048576"/>
+      <selection sqref="A1:U34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2717,11 +2725,4823 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331FAD02-2ECB-4DFB-AEEA-64D01B7F2EF6}">
+  <dimension ref="A1:AF35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="32" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B1" s="2">
+        <v>2018</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2">
+        <v>2019</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2">
+        <v>2020</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2">
+        <v>2022</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2">
+        <v>2018</v>
+      </c>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2">
+        <v>2019</v>
+      </c>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2">
+        <v>2020</v>
+      </c>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2">
+        <v>2021</v>
+      </c>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2">
+        <v>2022</v>
+      </c>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" t="s">
+        <v>3</v>
+      </c>
+      <c r="X2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <f>M3+O3</f>
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <f>N3+P3</f>
+        <v>86</v>
+      </c>
+      <c r="D3">
+        <f>S3+Q3</f>
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <f>T3+R3</f>
+        <v>70</v>
+      </c>
+      <c r="F3">
+        <f>U3+W3</f>
+        <v>19</v>
+      </c>
+      <c r="G3">
+        <f>V3+X3</f>
+        <v>66</v>
+      </c>
+      <c r="H3">
+        <f>Y3+AA3</f>
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <f>Z3+AB3</f>
+        <v>75</v>
+      </c>
+      <c r="J3">
+        <f>AC3+AE3</f>
+        <v>19</v>
+      </c>
+      <c r="K3">
+        <f>AD3+AF3</f>
+        <v>71</v>
+      </c>
+      <c r="M3">
+        <v>6</v>
+      </c>
+      <c r="N3">
+        <v>42</v>
+      </c>
+      <c r="O3">
+        <v>7</v>
+      </c>
+      <c r="P3">
+        <v>44</v>
+      </c>
+      <c r="Q3">
+        <v>6</v>
+      </c>
+      <c r="R3">
+        <v>41</v>
+      </c>
+      <c r="S3">
+        <v>5</v>
+      </c>
+      <c r="T3">
+        <v>29</v>
+      </c>
+      <c r="U3">
+        <v>11</v>
+      </c>
+      <c r="V3">
+        <v>36</v>
+      </c>
+      <c r="W3">
+        <v>8</v>
+      </c>
+      <c r="X3">
+        <v>30</v>
+      </c>
+      <c r="Y3">
+        <v>7</v>
+      </c>
+      <c r="Z3">
+        <v>41</v>
+      </c>
+      <c r="AA3">
+        <v>8</v>
+      </c>
+      <c r="AB3">
+        <v>34</v>
+      </c>
+      <c r="AC3">
+        <v>9</v>
+      </c>
+      <c r="AD3">
+        <v>39</v>
+      </c>
+      <c r="AE3">
+        <v>10</v>
+      </c>
+      <c r="AF3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V4" t="s">
+        <v>2</v>
+      </c>
+      <c r="W4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T5" t="s">
+        <v>5</v>
+      </c>
+      <c r="U5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W5" t="s">
+        <v>5</v>
+      </c>
+      <c r="X5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ref="B4:B35" si="0">M6+O6</f>
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C4:C35" si="1">N6+P6</f>
+        <v>47</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D4:D35" si="2">S6+Q6</f>
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E4:E35" si="3">T6+R6</f>
+        <v>46</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F4:F35" si="4">U6+W6</f>
+        <v>16</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G4:G35" si="5">V6+X6</f>
+        <v>46</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H4:H35" si="6">Y6+AA6</f>
+        <v>18</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I4:I35" si="7">Z6+AB6</f>
+        <v>41</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J4:J35" si="8">AC6+AE6</f>
+        <v>17</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K4:K35" si="9">AD6+AF6</f>
+        <v>41</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>29</v>
+      </c>
+      <c r="O6">
+        <v>8</v>
+      </c>
+      <c r="P6">
+        <v>18</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6">
+        <v>26</v>
+      </c>
+      <c r="S6">
+        <v>8</v>
+      </c>
+      <c r="T6">
+        <v>20</v>
+      </c>
+      <c r="U6">
+        <v>8</v>
+      </c>
+      <c r="V6">
+        <v>27</v>
+      </c>
+      <c r="W6">
+        <v>8</v>
+      </c>
+      <c r="X6">
+        <v>19</v>
+      </c>
+      <c r="Y6">
+        <v>10</v>
+      </c>
+      <c r="Z6">
+        <v>23</v>
+      </c>
+      <c r="AA6">
+        <v>8</v>
+      </c>
+      <c r="AB6">
+        <v>18</v>
+      </c>
+      <c r="AC6">
+        <v>8</v>
+      </c>
+      <c r="AD6">
+        <v>23</v>
+      </c>
+      <c r="AE6">
+        <v>9</v>
+      </c>
+      <c r="AF6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="5"/>
+        <v>41</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="7"/>
+        <v>47</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="8"/>
+        <v>17</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="9"/>
+        <v>45</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>26</v>
+      </c>
+      <c r="O7">
+        <v>10</v>
+      </c>
+      <c r="P7">
+        <v>15</v>
+      </c>
+      <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7">
+        <v>30</v>
+      </c>
+      <c r="S7">
+        <v>10</v>
+      </c>
+      <c r="T7">
+        <v>16</v>
+      </c>
+      <c r="U7">
+        <v>6</v>
+      </c>
+      <c r="V7">
+        <v>23</v>
+      </c>
+      <c r="W7">
+        <v>5</v>
+      </c>
+      <c r="X7">
+        <v>18</v>
+      </c>
+      <c r="Y7">
+        <v>10</v>
+      </c>
+      <c r="Z7">
+        <v>27</v>
+      </c>
+      <c r="AA7">
+        <v>7</v>
+      </c>
+      <c r="AB7">
+        <v>20</v>
+      </c>
+      <c r="AC7">
+        <v>11</v>
+      </c>
+      <c r="AD7">
+        <v>25</v>
+      </c>
+      <c r="AE7">
+        <v>6</v>
+      </c>
+      <c r="AF7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="5"/>
+        <v>37</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="7"/>
+        <v>37</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="9"/>
+        <v>34</v>
+      </c>
+      <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8">
+        <v>25</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <v>8</v>
+      </c>
+      <c r="Q8">
+        <v>4</v>
+      </c>
+      <c r="R8">
+        <v>25</v>
+      </c>
+      <c r="S8">
+        <v>2</v>
+      </c>
+      <c r="T8">
+        <v>8</v>
+      </c>
+      <c r="U8">
+        <v>4</v>
+      </c>
+      <c r="V8">
+        <v>27</v>
+      </c>
+      <c r="W8">
+        <v>4</v>
+      </c>
+      <c r="X8">
+        <v>10</v>
+      </c>
+      <c r="Y8">
+        <v>4</v>
+      </c>
+      <c r="Z8">
+        <v>27</v>
+      </c>
+      <c r="AA8">
+        <v>4</v>
+      </c>
+      <c r="AB8">
+        <v>10</v>
+      </c>
+      <c r="AC8">
+        <v>4</v>
+      </c>
+      <c r="AD8">
+        <v>24</v>
+      </c>
+      <c r="AE8">
+        <v>4</v>
+      </c>
+      <c r="AF8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="7"/>
+        <v>38</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="9"/>
+        <v>39</v>
+      </c>
+      <c r="M9">
+        <v>10</v>
+      </c>
+      <c r="N9">
+        <v>27</v>
+      </c>
+      <c r="O9">
+        <v>6</v>
+      </c>
+      <c r="P9">
+        <v>15</v>
+      </c>
+      <c r="Q9">
+        <v>10</v>
+      </c>
+      <c r="R9">
+        <v>26</v>
+      </c>
+      <c r="S9">
+        <v>8</v>
+      </c>
+      <c r="T9">
+        <v>15</v>
+      </c>
+      <c r="U9">
+        <v>12</v>
+      </c>
+      <c r="V9">
+        <v>23</v>
+      </c>
+      <c r="W9">
+        <v>12</v>
+      </c>
+      <c r="X9">
+        <v>12</v>
+      </c>
+      <c r="Y9">
+        <v>13</v>
+      </c>
+      <c r="Z9">
+        <v>24</v>
+      </c>
+      <c r="AA9">
+        <v>9</v>
+      </c>
+      <c r="AB9">
+        <v>14</v>
+      </c>
+      <c r="AC9">
+        <v>11</v>
+      </c>
+      <c r="AD9">
+        <v>25</v>
+      </c>
+      <c r="AE9">
+        <v>4</v>
+      </c>
+      <c r="AF9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="5"/>
+        <v>38</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="7"/>
+        <v>32</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="9"/>
+        <v>35</v>
+      </c>
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10">
+        <v>26</v>
+      </c>
+      <c r="O10">
+        <v>6</v>
+      </c>
+      <c r="P10">
+        <v>10</v>
+      </c>
+      <c r="Q10">
+        <v>5</v>
+      </c>
+      <c r="R10">
+        <v>25</v>
+      </c>
+      <c r="S10">
+        <v>6</v>
+      </c>
+      <c r="T10">
+        <v>15</v>
+      </c>
+      <c r="U10">
+        <v>3</v>
+      </c>
+      <c r="V10">
+        <v>28</v>
+      </c>
+      <c r="W10">
+        <v>3</v>
+      </c>
+      <c r="X10">
+        <v>10</v>
+      </c>
+      <c r="Y10">
+        <v>7</v>
+      </c>
+      <c r="Z10">
+        <v>22</v>
+      </c>
+      <c r="AA10">
+        <v>3</v>
+      </c>
+      <c r="AB10">
+        <v>10</v>
+      </c>
+      <c r="AC10">
+        <v>7</v>
+      </c>
+      <c r="AD10">
+        <v>23</v>
+      </c>
+      <c r="AE10">
+        <v>4</v>
+      </c>
+      <c r="AF10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>46</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="7"/>
+        <v>47</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="M11">
+        <v>8</v>
+      </c>
+      <c r="N11">
+        <v>23</v>
+      </c>
+      <c r="O11">
+        <v>7</v>
+      </c>
+      <c r="P11">
+        <v>16</v>
+      </c>
+      <c r="Q11">
+        <v>7</v>
+      </c>
+      <c r="R11">
+        <v>25</v>
+      </c>
+      <c r="S11">
+        <v>7</v>
+      </c>
+      <c r="T11">
+        <v>18</v>
+      </c>
+      <c r="U11">
+        <v>6</v>
+      </c>
+      <c r="V11">
+        <v>27</v>
+      </c>
+      <c r="W11">
+        <v>6</v>
+      </c>
+      <c r="X11">
+        <v>19</v>
+      </c>
+      <c r="Y11">
+        <v>6</v>
+      </c>
+      <c r="Z11">
+        <v>28</v>
+      </c>
+      <c r="AA11">
+        <v>4</v>
+      </c>
+      <c r="AB11">
+        <v>19</v>
+      </c>
+      <c r="AC11">
+        <v>5</v>
+      </c>
+      <c r="AD11">
+        <v>25</v>
+      </c>
+      <c r="AE11">
+        <v>3</v>
+      </c>
+      <c r="AF11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M12" t="s">
+        <v>5</v>
+      </c>
+      <c r="N12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O12" t="s">
+        <v>5</v>
+      </c>
+      <c r="P12" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>5</v>
+      </c>
+      <c r="R12" t="s">
+        <v>5</v>
+      </c>
+      <c r="S12" t="s">
+        <v>5</v>
+      </c>
+      <c r="T12" t="s">
+        <v>5</v>
+      </c>
+      <c r="U12" t="s">
+        <v>5</v>
+      </c>
+      <c r="V12" t="s">
+        <v>5</v>
+      </c>
+      <c r="W12" t="s">
+        <v>5</v>
+      </c>
+      <c r="X12" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>3</v>
+      </c>
+      <c r="R13" t="s">
+        <v>2</v>
+      </c>
+      <c r="S13" t="s">
+        <v>3</v>
+      </c>
+      <c r="T13" t="s">
+        <v>2</v>
+      </c>
+      <c r="U13" t="s">
+        <v>3</v>
+      </c>
+      <c r="V13" t="s">
+        <v>2</v>
+      </c>
+      <c r="W13" t="s">
+        <v>3</v>
+      </c>
+      <c r="X13" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>52</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="7"/>
+        <v>60</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="9"/>
+        <v>58</v>
+      </c>
+      <c r="M14">
+        <v>10</v>
+      </c>
+      <c r="N14">
+        <v>33</v>
+      </c>
+      <c r="O14">
+        <v>7</v>
+      </c>
+      <c r="P14">
+        <v>16</v>
+      </c>
+      <c r="Q14">
+        <v>10</v>
+      </c>
+      <c r="R14">
+        <v>33</v>
+      </c>
+      <c r="S14">
+        <v>7</v>
+      </c>
+      <c r="T14">
+        <v>16</v>
+      </c>
+      <c r="U14">
+        <v>8</v>
+      </c>
+      <c r="V14">
+        <v>36</v>
+      </c>
+      <c r="W14">
+        <v>11</v>
+      </c>
+      <c r="X14">
+        <v>16</v>
+      </c>
+      <c r="Y14">
+        <v>8</v>
+      </c>
+      <c r="Z14">
+        <v>44</v>
+      </c>
+      <c r="AA14">
+        <v>11</v>
+      </c>
+      <c r="AB14">
+        <v>16</v>
+      </c>
+      <c r="AC14">
+        <v>10</v>
+      </c>
+      <c r="AD14">
+        <v>38</v>
+      </c>
+      <c r="AE14">
+        <v>5</v>
+      </c>
+      <c r="AF14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>37</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="7"/>
+        <v>36</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="9"/>
+        <v>39</v>
+      </c>
+      <c r="M15">
+        <v>6</v>
+      </c>
+      <c r="N15">
+        <v>22</v>
+      </c>
+      <c r="O15">
+        <v>4</v>
+      </c>
+      <c r="P15">
+        <v>12</v>
+      </c>
+      <c r="Q15">
+        <v>6</v>
+      </c>
+      <c r="R15">
+        <v>25</v>
+      </c>
+      <c r="S15">
+        <v>7</v>
+      </c>
+      <c r="T15">
+        <v>12</v>
+      </c>
+      <c r="U15">
+        <v>3</v>
+      </c>
+      <c r="V15">
+        <v>27</v>
+      </c>
+      <c r="W15">
+        <v>7</v>
+      </c>
+      <c r="X15">
+        <v>10</v>
+      </c>
+      <c r="Y15">
+        <v>3</v>
+      </c>
+      <c r="Z15">
+        <v>27</v>
+      </c>
+      <c r="AA15">
+        <v>7</v>
+      </c>
+      <c r="AB15">
+        <v>9</v>
+      </c>
+      <c r="AC15">
+        <v>4</v>
+      </c>
+      <c r="AD15">
+        <v>28</v>
+      </c>
+      <c r="AE15">
+        <v>5</v>
+      </c>
+      <c r="AF15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>49</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="7"/>
+        <v>46</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="8"/>
+        <v>17</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="9"/>
+        <v>46</v>
+      </c>
+      <c r="M16">
+        <v>9</v>
+      </c>
+      <c r="N16">
+        <v>33</v>
+      </c>
+      <c r="O16">
+        <v>8</v>
+      </c>
+      <c r="P16">
+        <v>14</v>
+      </c>
+      <c r="Q16">
+        <v>11</v>
+      </c>
+      <c r="R16">
+        <v>32</v>
+      </c>
+      <c r="S16">
+        <v>9</v>
+      </c>
+      <c r="T16">
+        <v>15</v>
+      </c>
+      <c r="U16">
+        <v>8</v>
+      </c>
+      <c r="V16">
+        <v>35</v>
+      </c>
+      <c r="W16">
+        <v>6</v>
+      </c>
+      <c r="X16">
+        <v>14</v>
+      </c>
+      <c r="Y16">
+        <v>9</v>
+      </c>
+      <c r="Z16">
+        <v>35</v>
+      </c>
+      <c r="AA16">
+        <v>10</v>
+      </c>
+      <c r="AB16">
+        <v>11</v>
+      </c>
+      <c r="AC16">
+        <v>8</v>
+      </c>
+      <c r="AD16">
+        <v>35</v>
+      </c>
+      <c r="AE16">
+        <v>9</v>
+      </c>
+      <c r="AF16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="7"/>
+        <v>48</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="8"/>
+        <v>21</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="9"/>
+        <v>48</v>
+      </c>
+      <c r="M17">
+        <v>8</v>
+      </c>
+      <c r="N17">
+        <v>37</v>
+      </c>
+      <c r="O17">
+        <v>13</v>
+      </c>
+      <c r="P17">
+        <v>12</v>
+      </c>
+      <c r="Q17">
+        <v>12</v>
+      </c>
+      <c r="R17">
+        <v>34</v>
+      </c>
+      <c r="S17">
+        <v>9</v>
+      </c>
+      <c r="T17">
+        <v>16</v>
+      </c>
+      <c r="U17">
+        <v>13</v>
+      </c>
+      <c r="V17">
+        <v>33</v>
+      </c>
+      <c r="W17">
+        <v>11</v>
+      </c>
+      <c r="X17">
+        <v>15</v>
+      </c>
+      <c r="Y17">
+        <v>12</v>
+      </c>
+      <c r="Z17">
+        <v>33</v>
+      </c>
+      <c r="AA17">
+        <v>10</v>
+      </c>
+      <c r="AB17">
+        <v>15</v>
+      </c>
+      <c r="AC17">
+        <v>10</v>
+      </c>
+      <c r="AD17">
+        <v>35</v>
+      </c>
+      <c r="AE17">
+        <v>11</v>
+      </c>
+      <c r="AF17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>41</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="7"/>
+        <v>40</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="9"/>
+        <v>43</v>
+      </c>
+      <c r="M18">
+        <v>6</v>
+      </c>
+      <c r="N18">
+        <v>36</v>
+      </c>
+      <c r="O18">
+        <v>6</v>
+      </c>
+      <c r="P18">
+        <v>15</v>
+      </c>
+      <c r="Q18">
+        <v>6</v>
+      </c>
+      <c r="R18">
+        <v>37</v>
+      </c>
+      <c r="S18">
+        <v>5</v>
+      </c>
+      <c r="T18">
+        <v>17</v>
+      </c>
+      <c r="U18">
+        <v>9</v>
+      </c>
+      <c r="V18">
+        <v>31</v>
+      </c>
+      <c r="W18">
+        <v>7</v>
+      </c>
+      <c r="X18">
+        <v>10</v>
+      </c>
+      <c r="Y18">
+        <v>11</v>
+      </c>
+      <c r="Z18">
+        <v>31</v>
+      </c>
+      <c r="AA18">
+        <v>7</v>
+      </c>
+      <c r="AB18">
+        <v>9</v>
+      </c>
+      <c r="AC18">
+        <v>6</v>
+      </c>
+      <c r="AD18">
+        <v>31</v>
+      </c>
+      <c r="AE18">
+        <v>7</v>
+      </c>
+      <c r="AF18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>49</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="7"/>
+        <v>49</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="9"/>
+        <v>50</v>
+      </c>
+      <c r="M19">
+        <v>5</v>
+      </c>
+      <c r="N19">
+        <v>34</v>
+      </c>
+      <c r="O19">
+        <v>4</v>
+      </c>
+      <c r="P19">
+        <v>14</v>
+      </c>
+      <c r="Q19">
+        <v>4</v>
+      </c>
+      <c r="R19">
+        <v>35</v>
+      </c>
+      <c r="S19">
+        <v>6</v>
+      </c>
+      <c r="T19">
+        <v>13</v>
+      </c>
+      <c r="U19">
+        <v>4</v>
+      </c>
+      <c r="V19">
+        <v>36</v>
+      </c>
+      <c r="W19">
+        <v>6</v>
+      </c>
+      <c r="X19">
+        <v>13</v>
+      </c>
+      <c r="Y19">
+        <v>5</v>
+      </c>
+      <c r="Z19">
+        <v>35</v>
+      </c>
+      <c r="AA19">
+        <v>5</v>
+      </c>
+      <c r="AB19">
+        <v>14</v>
+      </c>
+      <c r="AC19">
+        <v>5</v>
+      </c>
+      <c r="AD19">
+        <v>36</v>
+      </c>
+      <c r="AE19">
+        <v>5</v>
+      </c>
+      <c r="AF19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="7"/>
+        <v>54</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="9"/>
+        <v>48</v>
+      </c>
+      <c r="M20">
+        <v>6</v>
+      </c>
+      <c r="N20">
+        <v>39</v>
+      </c>
+      <c r="O20">
+        <v>6</v>
+      </c>
+      <c r="P20">
+        <v>12</v>
+      </c>
+      <c r="Q20">
+        <v>6</v>
+      </c>
+      <c r="R20">
+        <v>39</v>
+      </c>
+      <c r="S20">
+        <v>6</v>
+      </c>
+      <c r="T20">
+        <v>12</v>
+      </c>
+      <c r="U20">
+        <v>3</v>
+      </c>
+      <c r="V20">
+        <v>40</v>
+      </c>
+      <c r="W20">
+        <v>5</v>
+      </c>
+      <c r="X20">
+        <v>14</v>
+      </c>
+      <c r="Y20">
+        <v>3</v>
+      </c>
+      <c r="Z20">
+        <v>40</v>
+      </c>
+      <c r="AA20">
+        <v>5</v>
+      </c>
+      <c r="AB20">
+        <v>14</v>
+      </c>
+      <c r="AC20">
+        <v>7</v>
+      </c>
+      <c r="AD20">
+        <v>33</v>
+      </c>
+      <c r="AE20">
+        <v>4</v>
+      </c>
+      <c r="AF20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="7"/>
+        <v>44</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="9"/>
+        <v>48</v>
+      </c>
+      <c r="M21">
+        <v>6</v>
+      </c>
+      <c r="N21">
+        <v>26</v>
+      </c>
+      <c r="O21">
+        <v>6</v>
+      </c>
+      <c r="P21">
+        <v>14</v>
+      </c>
+      <c r="Q21">
+        <v>5</v>
+      </c>
+      <c r="R21">
+        <v>26</v>
+      </c>
+      <c r="S21">
+        <v>6</v>
+      </c>
+      <c r="T21">
+        <v>14</v>
+      </c>
+      <c r="U21">
+        <v>5</v>
+      </c>
+      <c r="V21">
+        <v>28</v>
+      </c>
+      <c r="W21">
+        <v>6</v>
+      </c>
+      <c r="X21">
+        <v>14</v>
+      </c>
+      <c r="Y21">
+        <v>4</v>
+      </c>
+      <c r="Z21">
+        <v>31</v>
+      </c>
+      <c r="AA21">
+        <v>6</v>
+      </c>
+      <c r="AB21">
+        <v>13</v>
+      </c>
+      <c r="AC21">
+        <v>3</v>
+      </c>
+      <c r="AD21">
+        <v>36</v>
+      </c>
+      <c r="AE21">
+        <v>6</v>
+      </c>
+      <c r="AF21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="5"/>
+        <v>41</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="7"/>
+        <v>33</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="9"/>
+        <v>39</v>
+      </c>
+      <c r="M22">
+        <v>4</v>
+      </c>
+      <c r="N22">
+        <v>36</v>
+      </c>
+      <c r="O22">
+        <v>6</v>
+      </c>
+      <c r="P22">
+        <v>11</v>
+      </c>
+      <c r="Q22">
+        <v>4</v>
+      </c>
+      <c r="R22">
+        <v>28</v>
+      </c>
+      <c r="S22">
+        <v>4</v>
+      </c>
+      <c r="T22">
+        <v>8</v>
+      </c>
+      <c r="U22">
+        <v>5</v>
+      </c>
+      <c r="V22">
+        <v>33</v>
+      </c>
+      <c r="W22">
+        <v>6</v>
+      </c>
+      <c r="X22">
+        <v>8</v>
+      </c>
+      <c r="Y22">
+        <v>7</v>
+      </c>
+      <c r="Z22">
+        <v>27</v>
+      </c>
+      <c r="AA22">
+        <v>4</v>
+      </c>
+      <c r="AB22">
+        <v>6</v>
+      </c>
+      <c r="AC22">
+        <v>8</v>
+      </c>
+      <c r="AD22">
+        <v>29</v>
+      </c>
+      <c r="AE22">
+        <v>4</v>
+      </c>
+      <c r="AF22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>73</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="5"/>
+        <v>89</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="7"/>
+        <v>65</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="9"/>
+        <v>74</v>
+      </c>
+      <c r="M23">
+        <v>18</v>
+      </c>
+      <c r="N23">
+        <v>52</v>
+      </c>
+      <c r="O23">
+        <v>18</v>
+      </c>
+      <c r="P23">
+        <v>26</v>
+      </c>
+      <c r="Q23">
+        <v>13</v>
+      </c>
+      <c r="R23">
+        <v>48</v>
+      </c>
+      <c r="S23">
+        <v>13</v>
+      </c>
+      <c r="T23">
+        <v>25</v>
+      </c>
+      <c r="U23">
+        <v>16</v>
+      </c>
+      <c r="V23">
+        <v>67</v>
+      </c>
+      <c r="W23">
+        <v>17</v>
+      </c>
+      <c r="X23">
+        <v>22</v>
+      </c>
+      <c r="Y23">
+        <v>15</v>
+      </c>
+      <c r="Z23">
+        <v>47</v>
+      </c>
+      <c r="AA23">
+        <v>15</v>
+      </c>
+      <c r="AB23">
+        <v>18</v>
+      </c>
+      <c r="AC23">
+        <v>14</v>
+      </c>
+      <c r="AD23">
+        <v>53</v>
+      </c>
+      <c r="AE23">
+        <v>15</v>
+      </c>
+      <c r="AF23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="7"/>
+        <v>63</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="9"/>
+        <v>60</v>
+      </c>
+      <c r="M24">
+        <v>27</v>
+      </c>
+      <c r="N24">
+        <v>36</v>
+      </c>
+      <c r="O24">
+        <v>9</v>
+      </c>
+      <c r="P24">
+        <v>17</v>
+      </c>
+      <c r="Q24">
+        <v>17</v>
+      </c>
+      <c r="R24">
+        <v>45</v>
+      </c>
+      <c r="S24">
+        <v>9</v>
+      </c>
+      <c r="T24">
+        <v>18</v>
+      </c>
+      <c r="U24">
+        <v>13</v>
+      </c>
+      <c r="V24">
+        <v>44</v>
+      </c>
+      <c r="W24">
+        <v>10</v>
+      </c>
+      <c r="X24">
+        <v>16</v>
+      </c>
+      <c r="Y24">
+        <v>14</v>
+      </c>
+      <c r="Z24">
+        <v>44</v>
+      </c>
+      <c r="AA24">
+        <v>11</v>
+      </c>
+      <c r="AB24">
+        <v>19</v>
+      </c>
+      <c r="AC24">
+        <v>20</v>
+      </c>
+      <c r="AD24">
+        <v>41</v>
+      </c>
+      <c r="AE24">
+        <v>10</v>
+      </c>
+      <c r="AF24">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>69</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="7"/>
+        <v>65</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="9"/>
+        <v>71</v>
+      </c>
+      <c r="M25">
+        <v>8</v>
+      </c>
+      <c r="N25">
+        <v>51</v>
+      </c>
+      <c r="O25">
+        <v>5</v>
+      </c>
+      <c r="P25">
+        <v>17</v>
+      </c>
+      <c r="Q25">
+        <v>5</v>
+      </c>
+      <c r="R25">
+        <v>52</v>
+      </c>
+      <c r="S25">
+        <v>4</v>
+      </c>
+      <c r="T25">
+        <v>19</v>
+      </c>
+      <c r="U25">
+        <v>3</v>
+      </c>
+      <c r="V25">
+        <v>51</v>
+      </c>
+      <c r="W25">
+        <v>6</v>
+      </c>
+      <c r="X25">
+        <v>18</v>
+      </c>
+      <c r="Y25">
+        <v>4</v>
+      </c>
+      <c r="Z25">
+        <v>49</v>
+      </c>
+      <c r="AA25">
+        <v>3</v>
+      </c>
+      <c r="AB25">
+        <v>16</v>
+      </c>
+      <c r="AC25">
+        <v>5</v>
+      </c>
+      <c r="AD25">
+        <v>52</v>
+      </c>
+      <c r="AE25">
+        <v>2</v>
+      </c>
+      <c r="AF25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="5"/>
+        <v>78</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="7"/>
+        <v>78</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="9"/>
+        <v>80</v>
+      </c>
+      <c r="M26">
+        <v>7</v>
+      </c>
+      <c r="N26">
+        <v>62</v>
+      </c>
+      <c r="O26">
+        <v>10</v>
+      </c>
+      <c r="P26">
+        <v>22</v>
+      </c>
+      <c r="Q26">
+        <v>12</v>
+      </c>
+      <c r="R26">
+        <v>59</v>
+      </c>
+      <c r="S26">
+        <v>9</v>
+      </c>
+      <c r="T26">
+        <v>25</v>
+      </c>
+      <c r="U26">
+        <v>8</v>
+      </c>
+      <c r="V26">
+        <v>57</v>
+      </c>
+      <c r="W26">
+        <v>7</v>
+      </c>
+      <c r="X26">
+        <v>21</v>
+      </c>
+      <c r="Y26">
+        <v>8</v>
+      </c>
+      <c r="Z26">
+        <v>57</v>
+      </c>
+      <c r="AA26">
+        <v>7</v>
+      </c>
+      <c r="AB26">
+        <v>21</v>
+      </c>
+      <c r="AC26">
+        <v>9</v>
+      </c>
+      <c r="AD26">
+        <v>59</v>
+      </c>
+      <c r="AE26">
+        <v>7</v>
+      </c>
+      <c r="AF26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="5"/>
+        <v>63</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="7"/>
+        <v>68</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="9"/>
+        <v>61</v>
+      </c>
+      <c r="M27">
+        <v>10</v>
+      </c>
+      <c r="N27">
+        <v>44</v>
+      </c>
+      <c r="O27">
+        <v>10</v>
+      </c>
+      <c r="P27">
+        <v>19</v>
+      </c>
+      <c r="Q27">
+        <v>6</v>
+      </c>
+      <c r="R27">
+        <v>43</v>
+      </c>
+      <c r="S27">
+        <v>11</v>
+      </c>
+      <c r="T27">
+        <v>18</v>
+      </c>
+      <c r="U27">
+        <v>7</v>
+      </c>
+      <c r="V27">
+        <v>44</v>
+      </c>
+      <c r="W27">
+        <v>8</v>
+      </c>
+      <c r="X27">
+        <v>19</v>
+      </c>
+      <c r="Y27">
+        <v>6</v>
+      </c>
+      <c r="Z27">
+        <v>47</v>
+      </c>
+      <c r="AA27">
+        <v>5</v>
+      </c>
+      <c r="AB27">
+        <v>21</v>
+      </c>
+      <c r="AC27">
+        <v>7</v>
+      </c>
+      <c r="AD27">
+        <v>42</v>
+      </c>
+      <c r="AE27">
+        <v>6</v>
+      </c>
+      <c r="AF27">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="5"/>
+        <v>46</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="7"/>
+        <v>43</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="9"/>
+        <v>44</v>
+      </c>
+      <c r="M28">
+        <v>8</v>
+      </c>
+      <c r="N28">
+        <v>32</v>
+      </c>
+      <c r="O28">
+        <v>11</v>
+      </c>
+      <c r="P28">
+        <v>14</v>
+      </c>
+      <c r="Q28">
+        <v>13</v>
+      </c>
+      <c r="R28">
+        <v>28</v>
+      </c>
+      <c r="S28">
+        <v>8</v>
+      </c>
+      <c r="T28">
+        <v>17</v>
+      </c>
+      <c r="U28">
+        <v>13</v>
+      </c>
+      <c r="V28">
+        <v>28</v>
+      </c>
+      <c r="W28">
+        <v>7</v>
+      </c>
+      <c r="X28">
+        <v>18</v>
+      </c>
+      <c r="Y28">
+        <v>11</v>
+      </c>
+      <c r="Z28">
+        <v>29</v>
+      </c>
+      <c r="AA28">
+        <v>11</v>
+      </c>
+      <c r="AB28">
+        <v>14</v>
+      </c>
+      <c r="AC28">
+        <v>8</v>
+      </c>
+      <c r="AD28">
+        <v>32</v>
+      </c>
+      <c r="AE28">
+        <v>10</v>
+      </c>
+      <c r="AF28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="3"/>
+        <v>57</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="5"/>
+        <v>57</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="7"/>
+        <v>57</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="9"/>
+        <v>53</v>
+      </c>
+      <c r="M29">
+        <v>10</v>
+      </c>
+      <c r="N29">
+        <v>39</v>
+      </c>
+      <c r="O29">
+        <v>9</v>
+      </c>
+      <c r="P29">
+        <v>16</v>
+      </c>
+      <c r="Q29">
+        <v>7</v>
+      </c>
+      <c r="R29">
+        <v>41</v>
+      </c>
+      <c r="S29">
+        <v>8</v>
+      </c>
+      <c r="T29">
+        <v>16</v>
+      </c>
+      <c r="U29">
+        <v>8</v>
+      </c>
+      <c r="V29">
+        <v>39</v>
+      </c>
+      <c r="W29">
+        <v>6</v>
+      </c>
+      <c r="X29">
+        <v>18</v>
+      </c>
+      <c r="Y29">
+        <v>8</v>
+      </c>
+      <c r="Z29">
+        <v>39</v>
+      </c>
+      <c r="AA29">
+        <v>6</v>
+      </c>
+      <c r="AB29">
+        <v>18</v>
+      </c>
+      <c r="AC29">
+        <v>7</v>
+      </c>
+      <c r="AD29">
+        <v>36</v>
+      </c>
+      <c r="AE29">
+        <v>4</v>
+      </c>
+      <c r="AF29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="5"/>
+        <v>74</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="7"/>
+        <v>70</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="8"/>
+        <v>17</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="9"/>
+        <v>70</v>
+      </c>
+      <c r="M30">
+        <v>9</v>
+      </c>
+      <c r="N30">
+        <v>39</v>
+      </c>
+      <c r="O30">
+        <v>7</v>
+      </c>
+      <c r="P30">
+        <v>35</v>
+      </c>
+      <c r="Q30">
+        <v>8</v>
+      </c>
+      <c r="R30">
+        <v>40</v>
+      </c>
+      <c r="S30">
+        <v>12</v>
+      </c>
+      <c r="T30">
+        <v>25</v>
+      </c>
+      <c r="U30">
+        <v>10</v>
+      </c>
+      <c r="V30">
+        <v>38</v>
+      </c>
+      <c r="W30">
+        <v>8</v>
+      </c>
+      <c r="X30">
+        <v>36</v>
+      </c>
+      <c r="Y30">
+        <v>8</v>
+      </c>
+      <c r="Z30">
+        <v>42</v>
+      </c>
+      <c r="AA30">
+        <v>9</v>
+      </c>
+      <c r="AB30">
+        <v>28</v>
+      </c>
+      <c r="AC30">
+        <v>8</v>
+      </c>
+      <c r="AD30">
+        <v>42</v>
+      </c>
+      <c r="AE30">
+        <v>9</v>
+      </c>
+      <c r="AF30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="5"/>
+        <v>39</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="7"/>
+        <v>33</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="M31">
+        <v>10</v>
+      </c>
+      <c r="N31">
+        <v>23</v>
+      </c>
+      <c r="O31">
+        <v>8</v>
+      </c>
+      <c r="P31">
+        <v>13</v>
+      </c>
+      <c r="Q31">
+        <v>10</v>
+      </c>
+      <c r="R31">
+        <v>24</v>
+      </c>
+      <c r="S31">
+        <v>9</v>
+      </c>
+      <c r="T31">
+        <v>15</v>
+      </c>
+      <c r="U31">
+        <v>9</v>
+      </c>
+      <c r="V31">
+        <v>24</v>
+      </c>
+      <c r="W31">
+        <v>7</v>
+      </c>
+      <c r="X31">
+        <v>15</v>
+      </c>
+      <c r="Y31">
+        <v>11</v>
+      </c>
+      <c r="Z31">
+        <v>20</v>
+      </c>
+      <c r="AA31">
+        <v>9</v>
+      </c>
+      <c r="AB31">
+        <v>13</v>
+      </c>
+      <c r="AC31">
+        <v>8</v>
+      </c>
+      <c r="AD31">
+        <v>24</v>
+      </c>
+      <c r="AE31">
+        <v>7</v>
+      </c>
+      <c r="AF31">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="7"/>
+        <v>40</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="9"/>
+        <v>39</v>
+      </c>
+      <c r="M32">
+        <v>6</v>
+      </c>
+      <c r="N32">
+        <v>31</v>
+      </c>
+      <c r="O32">
+        <v>6</v>
+      </c>
+      <c r="P32">
+        <v>13</v>
+      </c>
+      <c r="Q32">
+        <v>7</v>
+      </c>
+      <c r="R32">
+        <v>32</v>
+      </c>
+      <c r="S32">
+        <v>7</v>
+      </c>
+      <c r="T32">
+        <v>13</v>
+      </c>
+      <c r="U32">
+        <v>8</v>
+      </c>
+      <c r="V32">
+        <v>29</v>
+      </c>
+      <c r="W32">
+        <v>5</v>
+      </c>
+      <c r="X32">
+        <v>11</v>
+      </c>
+      <c r="Y32">
+        <v>7</v>
+      </c>
+      <c r="Z32">
+        <v>29</v>
+      </c>
+      <c r="AA32">
+        <v>6</v>
+      </c>
+      <c r="AB32">
+        <v>11</v>
+      </c>
+      <c r="AC32">
+        <v>11</v>
+      </c>
+      <c r="AD32">
+        <v>27</v>
+      </c>
+      <c r="AE32">
+        <v>5</v>
+      </c>
+      <c r="AF32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="7"/>
+        <v>42</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="9"/>
+        <v>42</v>
+      </c>
+      <c r="M33">
+        <v>8</v>
+      </c>
+      <c r="N33">
+        <v>29</v>
+      </c>
+      <c r="O33">
+        <v>9</v>
+      </c>
+      <c r="P33">
+        <v>13</v>
+      </c>
+      <c r="Q33">
+        <v>7</v>
+      </c>
+      <c r="R33">
+        <v>28</v>
+      </c>
+      <c r="S33">
+        <v>10</v>
+      </c>
+      <c r="T33">
+        <v>9</v>
+      </c>
+      <c r="U33">
+        <v>6</v>
+      </c>
+      <c r="V33">
+        <v>27</v>
+      </c>
+      <c r="W33">
+        <v>10</v>
+      </c>
+      <c r="X33">
+        <v>9</v>
+      </c>
+      <c r="Y33">
+        <v>9</v>
+      </c>
+      <c r="Z33">
+        <v>28</v>
+      </c>
+      <c r="AA33">
+        <v>4</v>
+      </c>
+      <c r="AB33">
+        <v>14</v>
+      </c>
+      <c r="AC33">
+        <v>10</v>
+      </c>
+      <c r="AD33">
+        <v>27</v>
+      </c>
+      <c r="AE33">
+        <v>3</v>
+      </c>
+      <c r="AF33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="7"/>
+        <v>42</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="9"/>
+        <v>41</v>
+      </c>
+      <c r="M34">
+        <v>6</v>
+      </c>
+      <c r="N34">
+        <v>27</v>
+      </c>
+      <c r="O34">
+        <v>5</v>
+      </c>
+      <c r="P34">
+        <v>14</v>
+      </c>
+      <c r="Q34">
+        <v>6</v>
+      </c>
+      <c r="R34">
+        <v>27</v>
+      </c>
+      <c r="S34">
+        <v>5</v>
+      </c>
+      <c r="T34">
+        <v>14</v>
+      </c>
+      <c r="U34">
+        <v>6</v>
+      </c>
+      <c r="V34">
+        <v>27</v>
+      </c>
+      <c r="W34">
+        <v>3</v>
+      </c>
+      <c r="X34">
+        <v>13</v>
+      </c>
+      <c r="Y34">
+        <v>6</v>
+      </c>
+      <c r="Z34">
+        <v>27</v>
+      </c>
+      <c r="AA34">
+        <v>2</v>
+      </c>
+      <c r="AB34">
+        <v>15</v>
+      </c>
+      <c r="AC34">
+        <v>6</v>
+      </c>
+      <c r="AD34">
+        <v>26</v>
+      </c>
+      <c r="AE34">
+        <v>3</v>
+      </c>
+      <c r="AF34">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="5"/>
+        <v>41</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="7"/>
+        <v>49</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="9"/>
+        <v>49</v>
+      </c>
+      <c r="M35">
+        <v>7</v>
+      </c>
+      <c r="N35">
+        <v>27</v>
+      </c>
+      <c r="O35">
+        <v>2</v>
+      </c>
+      <c r="P35">
+        <v>12</v>
+      </c>
+      <c r="Q35">
+        <v>17</v>
+      </c>
+      <c r="R35">
+        <v>27</v>
+      </c>
+      <c r="S35">
+        <v>2</v>
+      </c>
+      <c r="T35">
+        <v>12</v>
+      </c>
+      <c r="U35">
+        <v>8</v>
+      </c>
+      <c r="V35">
+        <v>31</v>
+      </c>
+      <c r="W35">
+        <v>2</v>
+      </c>
+      <c r="X35">
+        <v>10</v>
+      </c>
+      <c r="Y35">
+        <v>5</v>
+      </c>
+      <c r="Z35">
+        <v>34</v>
+      </c>
+      <c r="AA35">
+        <v>4</v>
+      </c>
+      <c r="AB35">
+        <v>15</v>
+      </c>
+      <c r="AC35">
+        <v>8</v>
+      </c>
+      <c r="AD35">
+        <v>35</v>
+      </c>
+      <c r="AE35">
+        <v>4</v>
+      </c>
+      <c r="AF35">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8039BFCB-4DE1-4D66-AEF7-61E5215B8D10}">
+  <dimension ref="A1:K34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>86</v>
+      </c>
+      <c r="D2">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>70</v>
+      </c>
+      <c r="F2">
+        <v>19</v>
+      </c>
+      <c r="G2">
+        <v>66</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
+      <c r="I2">
+        <v>75</v>
+      </c>
+      <c r="J2">
+        <v>19</v>
+      </c>
+      <c r="K2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>47</v>
+      </c>
+      <c r="D5">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>46</v>
+      </c>
+      <c r="F5">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>46</v>
+      </c>
+      <c r="H5">
+        <v>18</v>
+      </c>
+      <c r="I5">
+        <v>41</v>
+      </c>
+      <c r="J5">
+        <v>17</v>
+      </c>
+      <c r="K5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>41</v>
+      </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>46</v>
+      </c>
+      <c r="F6">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>41</v>
+      </c>
+      <c r="H6">
+        <v>17</v>
+      </c>
+      <c r="I6">
+        <v>47</v>
+      </c>
+      <c r="J6">
+        <v>17</v>
+      </c>
+      <c r="K6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>33</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>33</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>37</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>37</v>
+      </c>
+      <c r="J7">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>42</v>
+      </c>
+      <c r="D8">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>41</v>
+      </c>
+      <c r="F8">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>35</v>
+      </c>
+      <c r="H8">
+        <v>22</v>
+      </c>
+      <c r="I8">
+        <v>38</v>
+      </c>
+      <c r="J8">
+        <v>15</v>
+      </c>
+      <c r="K8">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>40</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>38</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>32</v>
+      </c>
+      <c r="J9">
+        <v>11</v>
+      </c>
+      <c r="K9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>39</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>43</v>
+      </c>
+      <c r="F10">
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <v>46</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <v>47</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>49</v>
+      </c>
+      <c r="D13">
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>49</v>
+      </c>
+      <c r="F13">
+        <v>19</v>
+      </c>
+      <c r="G13">
+        <v>52</v>
+      </c>
+      <c r="H13">
+        <v>19</v>
+      </c>
+      <c r="I13">
+        <v>60</v>
+      </c>
+      <c r="J13">
+        <v>15</v>
+      </c>
+      <c r="K13">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>34</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>37</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>37</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>36</v>
+      </c>
+      <c r="J14">
+        <v>9</v>
+      </c>
+      <c r="K14">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>47</v>
+      </c>
+      <c r="D15">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>47</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>49</v>
+      </c>
+      <c r="H15">
+        <v>19</v>
+      </c>
+      <c r="I15">
+        <v>46</v>
+      </c>
+      <c r="J15">
+        <v>17</v>
+      </c>
+      <c r="K15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>49</v>
+      </c>
+      <c r="D16">
+        <v>21</v>
+      </c>
+      <c r="E16">
+        <v>50</v>
+      </c>
+      <c r="F16">
+        <v>24</v>
+      </c>
+      <c r="G16">
+        <v>48</v>
+      </c>
+      <c r="H16">
+        <v>22</v>
+      </c>
+      <c r="I16">
+        <v>48</v>
+      </c>
+      <c r="J16">
+        <v>21</v>
+      </c>
+      <c r="K16">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>51</v>
+      </c>
+      <c r="D17">
+        <v>11</v>
+      </c>
+      <c r="E17">
+        <v>54</v>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
+      <c r="G17">
+        <v>41</v>
+      </c>
+      <c r="H17">
+        <v>18</v>
+      </c>
+      <c r="I17">
+        <v>40</v>
+      </c>
+      <c r="J17">
+        <v>13</v>
+      </c>
+      <c r="K17">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>48</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>48</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+      <c r="G18">
+        <v>49</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>49</v>
+      </c>
+      <c r="J18">
+        <v>10</v>
+      </c>
+      <c r="K18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>51</v>
+      </c>
+      <c r="D19">
+        <v>12</v>
+      </c>
+      <c r="E19">
+        <v>51</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>54</v>
+      </c>
+      <c r="H19">
+        <v>8</v>
+      </c>
+      <c r="I19">
+        <v>54</v>
+      </c>
+      <c r="J19">
+        <v>11</v>
+      </c>
+      <c r="K19">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>40</v>
+      </c>
+      <c r="D20">
+        <v>11</v>
+      </c>
+      <c r="E20">
+        <v>40</v>
+      </c>
+      <c r="F20">
+        <v>11</v>
+      </c>
+      <c r="G20">
+        <v>42</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="I20">
+        <v>44</v>
+      </c>
+      <c r="J20">
+        <v>9</v>
+      </c>
+      <c r="K20">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>47</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>36</v>
+      </c>
+      <c r="F21">
+        <v>11</v>
+      </c>
+      <c r="G21">
+        <v>41</v>
+      </c>
+      <c r="H21">
+        <v>11</v>
+      </c>
+      <c r="I21">
+        <v>33</v>
+      </c>
+      <c r="J21">
+        <v>12</v>
+      </c>
+      <c r="K21">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>36</v>
+      </c>
+      <c r="C22">
+        <v>78</v>
+      </c>
+      <c r="D22">
+        <v>26</v>
+      </c>
+      <c r="E22">
+        <v>73</v>
+      </c>
+      <c r="F22">
+        <v>33</v>
+      </c>
+      <c r="G22">
+        <v>89</v>
+      </c>
+      <c r="H22">
+        <v>30</v>
+      </c>
+      <c r="I22">
+        <v>65</v>
+      </c>
+      <c r="J22">
+        <v>29</v>
+      </c>
+      <c r="K22">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>36</v>
+      </c>
+      <c r="C23">
+        <v>53</v>
+      </c>
+      <c r="D23">
+        <v>26</v>
+      </c>
+      <c r="E23">
+        <v>63</v>
+      </c>
+      <c r="F23">
+        <v>23</v>
+      </c>
+      <c r="G23">
+        <v>60</v>
+      </c>
+      <c r="H23">
+        <v>25</v>
+      </c>
+      <c r="I23">
+        <v>63</v>
+      </c>
+      <c r="J23">
+        <v>30</v>
+      </c>
+      <c r="K23">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>68</v>
+      </c>
+      <c r="D24">
+        <v>9</v>
+      </c>
+      <c r="E24">
+        <v>71</v>
+      </c>
+      <c r="F24">
+        <v>9</v>
+      </c>
+      <c r="G24">
+        <v>69</v>
+      </c>
+      <c r="H24">
+        <v>7</v>
+      </c>
+      <c r="I24">
+        <v>65</v>
+      </c>
+      <c r="J24">
+        <v>7</v>
+      </c>
+      <c r="K24">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>17</v>
+      </c>
+      <c r="C25">
+        <v>84</v>
+      </c>
+      <c r="D25">
+        <v>21</v>
+      </c>
+      <c r="E25">
+        <v>84</v>
+      </c>
+      <c r="F25">
+        <v>15</v>
+      </c>
+      <c r="G25">
+        <v>78</v>
+      </c>
+      <c r="H25">
+        <v>15</v>
+      </c>
+      <c r="I25">
+        <v>78</v>
+      </c>
+      <c r="J25">
+        <v>16</v>
+      </c>
+      <c r="K25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>20</v>
+      </c>
+      <c r="C26">
+        <v>63</v>
+      </c>
+      <c r="D26">
+        <v>17</v>
+      </c>
+      <c r="E26">
+        <v>61</v>
+      </c>
+      <c r="F26">
+        <v>15</v>
+      </c>
+      <c r="G26">
+        <v>63</v>
+      </c>
+      <c r="H26">
+        <v>11</v>
+      </c>
+      <c r="I26">
+        <v>68</v>
+      </c>
+      <c r="J26">
+        <v>13</v>
+      </c>
+      <c r="K26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>19</v>
+      </c>
+      <c r="C27">
+        <v>46</v>
+      </c>
+      <c r="D27">
+        <v>21</v>
+      </c>
+      <c r="E27">
+        <v>45</v>
+      </c>
+      <c r="F27">
+        <v>20</v>
+      </c>
+      <c r="G27">
+        <v>46</v>
+      </c>
+      <c r="H27">
+        <v>22</v>
+      </c>
+      <c r="I27">
+        <v>43</v>
+      </c>
+      <c r="J27">
+        <v>18</v>
+      </c>
+      <c r="K27">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>19</v>
+      </c>
+      <c r="C28">
+        <v>55</v>
+      </c>
+      <c r="D28">
+        <v>15</v>
+      </c>
+      <c r="E28">
+        <v>57</v>
+      </c>
+      <c r="F28">
+        <v>14</v>
+      </c>
+      <c r="G28">
+        <v>57</v>
+      </c>
+      <c r="H28">
+        <v>14</v>
+      </c>
+      <c r="I28">
+        <v>57</v>
+      </c>
+      <c r="J28">
+        <v>11</v>
+      </c>
+      <c r="K28">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>16</v>
+      </c>
+      <c r="C29">
+        <v>74</v>
+      </c>
+      <c r="D29">
+        <v>20</v>
+      </c>
+      <c r="E29">
+        <v>65</v>
+      </c>
+      <c r="F29">
+        <v>18</v>
+      </c>
+      <c r="G29">
+        <v>74</v>
+      </c>
+      <c r="H29">
+        <v>17</v>
+      </c>
+      <c r="I29">
+        <v>70</v>
+      </c>
+      <c r="J29">
+        <v>17</v>
+      </c>
+      <c r="K29">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>18</v>
+      </c>
+      <c r="C30">
+        <v>36</v>
+      </c>
+      <c r="D30">
+        <v>19</v>
+      </c>
+      <c r="E30">
+        <v>39</v>
+      </c>
+      <c r="F30">
+        <v>16</v>
+      </c>
+      <c r="G30">
+        <v>39</v>
+      </c>
+      <c r="H30">
+        <v>20</v>
+      </c>
+      <c r="I30">
+        <v>33</v>
+      </c>
+      <c r="J30">
+        <v>15</v>
+      </c>
+      <c r="K30">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <v>44</v>
+      </c>
+      <c r="D31">
+        <v>14</v>
+      </c>
+      <c r="E31">
+        <v>45</v>
+      </c>
+      <c r="F31">
+        <v>13</v>
+      </c>
+      <c r="G31">
+        <v>40</v>
+      </c>
+      <c r="H31">
+        <v>13</v>
+      </c>
+      <c r="I31">
+        <v>40</v>
+      </c>
+      <c r="J31">
+        <v>16</v>
+      </c>
+      <c r="K31">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <v>17</v>
+      </c>
+      <c r="C32">
+        <v>42</v>
+      </c>
+      <c r="D32">
+        <v>17</v>
+      </c>
+      <c r="E32">
+        <v>37</v>
+      </c>
+      <c r="F32">
+        <v>16</v>
+      </c>
+      <c r="G32">
+        <v>36</v>
+      </c>
+      <c r="H32">
+        <v>13</v>
+      </c>
+      <c r="I32">
+        <v>42</v>
+      </c>
+      <c r="J32">
+        <v>13</v>
+      </c>
+      <c r="K32">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>41</v>
+      </c>
+      <c r="D33">
+        <v>11</v>
+      </c>
+      <c r="E33">
+        <v>41</v>
+      </c>
+      <c r="F33">
+        <v>9</v>
+      </c>
+      <c r="G33">
+        <v>40</v>
+      </c>
+      <c r="H33">
+        <v>8</v>
+      </c>
+      <c r="I33">
+        <v>42</v>
+      </c>
+      <c r="J33">
+        <v>9</v>
+      </c>
+      <c r="K33">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>39</v>
+      </c>
+      <c r="D34">
+        <v>19</v>
+      </c>
+      <c r="E34">
+        <v>39</v>
+      </c>
+      <c r="F34">
+        <v>10</v>
+      </c>
+      <c r="G34">
+        <v>41</v>
+      </c>
+      <c r="H34">
+        <v>9</v>
+      </c>
+      <c r="I34">
+        <v>49</v>
+      </c>
+      <c r="J34">
+        <v>12</v>
+      </c>
+      <c r="K34">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA542F5E-79B6-4E94-A0D9-186A41F6B21B}">
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B4" sqref="B4:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3720,7 +8540,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D79F363-7D4E-4BC0-817B-578A9736A2BD}">
   <dimension ref="A1:I34"/>
   <sheetViews>
@@ -4732,11 +9552,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70FD8B95-D101-4F38-9C25-BA82133AAEC0}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>